<commit_message>
observations and small fix
</commit_message>
<xml_diff>
--- a/Output/25_observations.xlsx
+++ b/Output/25_observations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Master_Thesis\VS_Project\N_Body\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F4A9366-F2EC-4381-8D12-D0FCC7DCDB62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C4A1766-CC93-4372-BEA8-F6D5F9006848}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-30828" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -509,10 +509,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B7400D3-4408-4AB0-A4E0-D2D392275FE0}">
-  <dimension ref="A1:O5"/>
+  <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -711,6 +711,88 @@
       <c r="F5">
         <v>668</v>
       </c>
+      <c r="G5">
+        <v>7461</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>223</v>
+      </c>
+      <c r="J5">
+        <v>10</v>
+      </c>
+      <c r="K5">
+        <v>2063</v>
+      </c>
+      <c r="L5">
+        <v>623</v>
+      </c>
+      <c r="M5">
+        <v>599</v>
+      </c>
+      <c r="N5">
+        <v>3519</v>
+      </c>
+      <c r="O5">
+        <v>3295</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>180</v>
+      </c>
+      <c r="B6">
+        <v>10000</v>
+      </c>
+      <c r="C6">
+        <v>27</v>
+      </c>
+      <c r="D6">
+        <v>262</v>
+      </c>
+      <c r="E6">
+        <v>17598</v>
+      </c>
+      <c r="F6">
+        <v>642</v>
+      </c>
+      <c r="G6">
+        <v>18571</v>
+      </c>
+      <c r="H6">
+        <v>24</v>
+      </c>
+      <c r="I6">
+        <v>343</v>
+      </c>
+      <c r="J6">
+        <v>18</v>
+      </c>
+      <c r="K6">
+        <v>5645</v>
+      </c>
+      <c r="L6">
+        <v>903</v>
+      </c>
+      <c r="M6">
+        <v>540</v>
+      </c>
+      <c r="N6">
+        <v>7473</v>
+      </c>
+      <c r="O6">
+        <v>7106</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>180</v>
+      </c>
+      <c r="B7">
+        <v>25000</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
remove stars outside vision more data
</commit_message>
<xml_diff>
--- a/Output/25_observations.xlsx
+++ b/Output/25_observations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Master_Thesis\VS_Project\N_Body\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{676D626D-3B61-4A06-8C43-C806944249EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA2AF815-A004-4BBF-9CED-0BBBD29701FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -118,7 +118,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -126,8 +126,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -140,6 +147,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -150,10 +162,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -162,8 +175,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Gut" xfId="1" builtinId="26"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -516,10 +531,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B7400D3-4408-4AB0-A4E0-D2D392275FE0}">
-  <dimension ref="A1:O31"/>
+  <dimension ref="A1:Q31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -537,9 +552,10 @@
     <col min="13" max="13" width="22.85546875" customWidth="1"/>
     <col min="14" max="14" width="13.85546875" customWidth="1"/>
     <col min="15" max="15" width="13" customWidth="1"/>
+    <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C1" s="3" t="s">
         <v>17</v>
       </c>
@@ -558,7 +574,7 @@
       <c r="N1" s="3"/>
       <c r="O1" s="3"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -605,7 +621,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>180</v>
       </c>
@@ -651,8 +667,15 @@
       <c r="O3">
         <v>1680</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="P3">
+        <f>0.000381057258287357*0.03</f>
+        <v>1.143171774862071E-5</v>
+      </c>
+      <c r="Q3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>180</v>
       </c>
@@ -698,8 +721,12 @@
       <c r="O4" s="2">
         <v>2226</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P4">
+        <f>0.000381057258287357*0.03</f>
+        <v>1.143171774862071E-5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>180</v>
       </c>
@@ -745,8 +772,12 @@
       <c r="O5">
         <v>3295</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P5">
+        <f>0.000381057258287357*0.03</f>
+        <v>1.143171774862071E-5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>180</v>
       </c>
@@ -792,8 +823,12 @@
       <c r="O6">
         <v>7106</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P6">
+        <f>0.000381057258287357*0.03</f>
+        <v>1.143171774862071E-5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>180</v>
       </c>
@@ -839,8 +874,12 @@
       <c r="O7">
         <v>17259</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P7">
+        <f>0.000381057258287357*0.03</f>
+        <v>1.143171774862071E-5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>25</v>
       </c>
@@ -886,8 +925,12 @@
       <c r="O9">
         <v>18247</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P9">
+        <f>0.000381057258287357*0.03</f>
+        <v>1.143171774862071E-5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>25</v>
       </c>
@@ -933,8 +976,12 @@
       <c r="O10">
         <v>18775</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P10">
+        <f>0.000381057258287357*0.03</f>
+        <v>1.143171774862071E-5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>25</v>
       </c>
@@ -980,8 +1027,12 @@
       <c r="O11">
         <v>19641</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P11">
+        <f>0.000381057258287357*0.03</f>
+        <v>1.143171774862071E-5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>25</v>
       </c>
@@ -1027,8 +1078,12 @@
       <c r="O12">
         <v>23045</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P12">
+        <f>0.000381057258287357*0.03</f>
+        <v>1.143171774862071E-5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>25</v>
       </c>
@@ -1074,8 +1129,12 @@
       <c r="O13">
         <v>31775</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P13">
+        <f>0.000381057258287357*0.03</f>
+        <v>1.143171774862071E-5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>10</v>
       </c>
@@ -1121,8 +1180,12 @@
       <c r="O15">
         <v>40934</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P15">
+        <f>0.000381057258287357*0.03</f>
+        <v>1.143171774862071E-5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>10</v>
       </c>
@@ -1168,8 +1231,12 @@
       <c r="O16">
         <v>41270</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P16">
+        <f>0.000381057258287357*0.03</f>
+        <v>1.143171774862071E-5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>10</v>
       </c>
@@ -1215,56 +1282,298 @@
       <c r="O17">
         <v>41922</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P17">
+        <f>0.000381057258287357*0.03</f>
+        <v>1.143171774862071E-5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>10</v>
       </c>
       <c r="B18">
         <v>10000</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19">
+      <c r="C18">
+        <v>321</v>
+      </c>
+      <c r="D18">
+        <v>267</v>
+      </c>
+      <c r="E18">
+        <v>17633</v>
+      </c>
+      <c r="F18">
+        <v>47248</v>
+      </c>
+      <c r="G18">
+        <v>65469</v>
+      </c>
+      <c r="H18">
+        <v>13</v>
+      </c>
+      <c r="I18">
+        <v>655</v>
+      </c>
+      <c r="J18">
+        <v>262</v>
+      </c>
+      <c r="K18">
+        <v>6718</v>
+      </c>
+      <c r="L18">
+        <v>1091</v>
+      </c>
+      <c r="M18">
+        <v>36948</v>
+      </c>
+      <c r="N18">
+        <v>45687</v>
+      </c>
+      <c r="O18">
+        <v>45019</v>
+      </c>
+      <c r="P18">
+        <f>0.000381057258287357*0.03</f>
+        <v>1.143171774862071E-5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
         <v>10</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="4">
         <v>25000</v>
       </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21">
+      <c r="C19" s="4">
+        <v>695</v>
+      </c>
+      <c r="D19" s="4">
+        <v>515</v>
+      </c>
+      <c r="E19" s="4">
+        <v>39917</v>
+      </c>
+      <c r="F19" s="4">
+        <v>47055</v>
+      </c>
+      <c r="G19" s="4">
+        <v>88182</v>
+      </c>
+      <c r="H19" s="4">
+        <v>76</v>
+      </c>
+      <c r="I19" s="4">
+        <v>382</v>
+      </c>
+      <c r="J19" s="4">
+        <v>467</v>
+      </c>
+      <c r="K19" s="4">
+        <v>14442</v>
+      </c>
+      <c r="L19" s="4">
+        <v>913</v>
+      </c>
+      <c r="M19" s="4">
+        <v>29726</v>
+      </c>
+      <c r="N19" s="4">
+        <v>51341</v>
+      </c>
+      <c r="O19" s="4">
+        <v>50853</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
         <v>5</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="4">
         <v>640</v>
       </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22">
+      <c r="C21" s="4">
+        <v>28</v>
+      </c>
+      <c r="D21" s="4">
+        <v>18</v>
+      </c>
+      <c r="E21" s="4">
+        <v>1310</v>
+      </c>
+      <c r="F21" s="4">
+        <v>67618</v>
+      </c>
+      <c r="G21" s="4">
+        <v>68974</v>
+      </c>
+      <c r="H21" s="4">
+        <v>0</v>
+      </c>
+      <c r="I21" s="4">
+        <v>1063</v>
+      </c>
+      <c r="J21" s="4">
+        <v>35</v>
+      </c>
+      <c r="K21" s="4">
+        <v>552</v>
+      </c>
+      <c r="L21" s="4">
+        <v>429</v>
+      </c>
+      <c r="M21" s="4">
+        <v>55958</v>
+      </c>
+      <c r="N21" s="4">
+        <v>58037</v>
+      </c>
+      <c r="O21" s="4">
+        <v>56974</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
         <v>5</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="4">
         <v>1600</v>
       </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23">
+      <c r="C22" s="4">
+        <v>61</v>
+      </c>
+      <c r="D22" s="4">
+        <v>28</v>
+      </c>
+      <c r="E22" s="4">
+        <v>2749</v>
+      </c>
+      <c r="F22" s="4">
+        <v>67696</v>
+      </c>
+      <c r="G22" s="4">
+        <v>70534</v>
+      </c>
+      <c r="H22" s="4">
+        <v>2</v>
+      </c>
+      <c r="I22" s="4">
+        <v>907</v>
+      </c>
+      <c r="J22" s="4">
+        <v>89</v>
+      </c>
+      <c r="K22" s="4">
+        <v>1280</v>
+      </c>
+      <c r="L22" s="4">
+        <v>533</v>
+      </c>
+      <c r="M22" s="4">
+        <v>55683</v>
+      </c>
+      <c r="N22" s="4">
+        <v>58494</v>
+      </c>
+      <c r="O22" s="4">
+        <v>57585</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
         <v>5</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="4">
         <v>4000</v>
       </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C23" s="4">
+        <v>138</v>
+      </c>
+      <c r="D23" s="4">
+        <v>83</v>
+      </c>
+      <c r="E23" s="4">
+        <v>6434</v>
+      </c>
+      <c r="F23" s="4">
+        <v>67310</v>
+      </c>
+      <c r="G23" s="4">
+        <v>73965</v>
+      </c>
+      <c r="H23" s="4">
+        <v>5</v>
+      </c>
+      <c r="I23" s="4">
+        <v>1389</v>
+      </c>
+      <c r="J23" s="4">
+        <v>156</v>
+      </c>
+      <c r="K23" s="4">
+        <v>2647</v>
+      </c>
+      <c r="L23" s="4">
+        <v>764</v>
+      </c>
+      <c r="M23" s="4">
+        <v>53889</v>
+      </c>
+      <c r="N23" s="4">
+        <v>58850</v>
+      </c>
+      <c r="O23" s="4">
+        <v>57456</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>5</v>
       </c>
       <c r="B24">
         <v>10000</v>
       </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C24">
+        <v>225</v>
+      </c>
+      <c r="D24" s="4">
+        <v>267</v>
+      </c>
+      <c r="E24" s="4">
+        <v>16686</v>
+      </c>
+      <c r="F24" s="4">
+        <v>66949</v>
+      </c>
+      <c r="G24" s="4">
+        <v>84127</v>
+      </c>
+      <c r="H24" s="4">
+        <v>25</v>
+      </c>
+      <c r="I24" s="4">
+        <v>709</v>
+      </c>
+      <c r="J24" s="4">
+        <v>238</v>
+      </c>
+      <c r="K24" s="4">
+        <v>6525</v>
+      </c>
+      <c r="L24" s="4">
+        <v>1316</v>
+      </c>
+      <c r="M24" s="4">
+        <v>52124</v>
+      </c>
+      <c r="N24" s="4">
+        <v>60937</v>
+      </c>
+      <c r="O24" s="4">
+        <v>60203</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>5</v>
       </c>
@@ -1272,7 +1581,7 @@
         <v>25000</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>0</v>
       </c>
@@ -1280,7 +1589,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>0</v>
       </c>
@@ -1288,7 +1597,7 @@
         <v>1600</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>0</v>
       </c>
@@ -1296,7 +1605,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>0</v>
       </c>
@@ -1304,7 +1613,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>0</v>
       </c>
@@ -1318,5 +1627,6 @@
     <mergeCell ref="H1:O1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
25 data project done
</commit_message>
<xml_diff>
--- a/Output/25_observations.xlsx
+++ b/Output/25_observations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Master_Thesis\VS_Project\N_Body\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC87832A-7656-4E09-9F3F-48DA0987E61D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DF105BD-43A9-4951-84C1-93E0AD06E767}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -134,18 +134,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -164,15 +158,14 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -534,7 +527,7 @@
   <dimension ref="A1:Q31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31:XFD31"/>
+      <selection activeCell="A18" sqref="A18:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -556,23 +549,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4" t="s">
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -621,57 +614,57 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="3" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
         <v>180</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="2">
         <v>640</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="2">
         <v>2</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="2">
         <v>15</v>
       </c>
-      <c r="E3">
-        <v>1350</v>
-      </c>
-      <c r="F3">
-        <v>713</v>
-      </c>
-      <c r="G3">
-        <v>2080</v>
-      </c>
-      <c r="H3">
+      <c r="E3" s="2">
+        <v>1311</v>
+      </c>
+      <c r="F3" s="2">
+        <v>712</v>
+      </c>
+      <c r="G3" s="2">
+        <v>2040</v>
+      </c>
+      <c r="H3" s="2">
         <v>0</v>
       </c>
-      <c r="I3">
-        <v>222</v>
-      </c>
-      <c r="J3">
+      <c r="I3" s="2">
+        <v>221</v>
+      </c>
+      <c r="J3" s="2">
         <v>3</v>
       </c>
-      <c r="K3">
-        <v>725</v>
-      </c>
-      <c r="L3">
-        <v>273</v>
-      </c>
-      <c r="M3">
-        <v>679</v>
-      </c>
-      <c r="N3">
-        <v>1902</v>
-      </c>
-      <c r="O3">
-        <v>1680</v>
-      </c>
-      <c r="P3">
+      <c r="K3" s="2">
+        <v>716</v>
+      </c>
+      <c r="L3" s="2">
+        <v>250</v>
+      </c>
+      <c r="M3" s="2">
+        <v>672</v>
+      </c>
+      <c r="N3" s="2">
+        <v>1862</v>
+      </c>
+      <c r="O3" s="2">
+        <v>1641</v>
+      </c>
+      <c r="P3" s="2">
         <f>0.000381057258287357*0.03</f>
         <v>1.143171774862071E-5</v>
       </c>
-      <c r="Q3">
+      <c r="Q3" s="2">
         <v>200</v>
       </c>
     </row>
@@ -683,1175 +676,1175 @@
         <v>1600</v>
       </c>
       <c r="C4" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D4" s="2">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E4" s="2">
-        <v>2864</v>
+        <v>2758</v>
       </c>
       <c r="F4" s="2">
-        <v>687</v>
+        <v>701</v>
       </c>
       <c r="G4" s="2">
-        <v>3571</v>
+        <v>3482</v>
       </c>
       <c r="H4" s="2">
         <v>0</v>
       </c>
       <c r="I4" s="2">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="J4" s="2">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="K4" s="2">
-        <v>1202</v>
+        <v>1135</v>
       </c>
       <c r="L4" s="2">
-        <v>389</v>
+        <v>599</v>
       </c>
       <c r="M4" s="2">
-        <v>631</v>
+        <v>652</v>
       </c>
       <c r="N4" s="2">
-        <v>2479</v>
+        <v>2466</v>
       </c>
       <c r="O4" s="2">
-        <v>2226</v>
-      </c>
-      <c r="P4">
+        <v>2212</v>
+      </c>
+      <c r="P4" s="2">
         <f>0.000381057258287357*0.03</f>
         <v>1.143171774862071E-5</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="5" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
         <v>180</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="2">
         <v>4000</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="2">
         <v>13</v>
       </c>
-      <c r="D5">
-        <v>109</v>
-      </c>
-      <c r="E5">
-        <v>6670</v>
-      </c>
-      <c r="F5">
+      <c r="D5" s="2">
+        <v>102</v>
+      </c>
+      <c r="E5" s="2">
+        <v>6419</v>
+      </c>
+      <c r="F5" s="2">
         <v>669</v>
       </c>
-      <c r="G5">
-        <v>7461</v>
-      </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-      <c r="I5">
-        <v>223</v>
-      </c>
-      <c r="J5">
+      <c r="G5" s="2">
+        <v>7203</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0</v>
+      </c>
+      <c r="I5" s="2">
+        <v>194</v>
+      </c>
+      <c r="J5" s="2">
         <v>10</v>
       </c>
-      <c r="K5">
-        <v>2063</v>
-      </c>
-      <c r="L5">
-        <v>623</v>
-      </c>
-      <c r="M5">
+      <c r="K5" s="2">
+        <v>2003</v>
+      </c>
+      <c r="L5" s="2">
         <v>599</v>
       </c>
-      <c r="N5">
-        <v>3519</v>
-      </c>
-      <c r="O5">
-        <v>3295</v>
-      </c>
-      <c r="P5">
+      <c r="M5" s="2">
+        <v>599</v>
+      </c>
+      <c r="N5" s="2">
+        <v>3405</v>
+      </c>
+      <c r="O5" s="2">
+        <v>3211</v>
+      </c>
+      <c r="P5" s="2">
         <f>0.000381057258287357*0.03</f>
         <v>1.143171774862071E-5</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="6" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
         <v>180</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="2">
         <v>10000</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="2">
         <v>27</v>
       </c>
-      <c r="D6">
-        <v>302</v>
-      </c>
-      <c r="E6">
-        <v>17598</v>
-      </c>
-      <c r="F6">
+      <c r="D6" s="2">
+        <v>270</v>
+      </c>
+      <c r="E6" s="2">
+        <v>16679</v>
+      </c>
+      <c r="F6" s="2">
         <v>644</v>
       </c>
-      <c r="G6">
-        <v>18571</v>
-      </c>
-      <c r="H6">
-        <v>24</v>
-      </c>
-      <c r="I6">
-        <v>343</v>
-      </c>
-      <c r="J6">
+      <c r="G6" s="2">
+        <v>17620</v>
+      </c>
+      <c r="H6" s="2">
+        <v>16</v>
+      </c>
+      <c r="I6" s="2">
+        <v>152</v>
+      </c>
+      <c r="J6" s="2">
         <v>18</v>
       </c>
-      <c r="K6">
-        <v>5645</v>
-      </c>
-      <c r="L6">
-        <v>903</v>
-      </c>
-      <c r="M6">
+      <c r="K6" s="2">
+        <v>5342</v>
+      </c>
+      <c r="L6" s="2">
+        <v>910</v>
+      </c>
+      <c r="M6" s="2">
         <v>540</v>
       </c>
-      <c r="N6">
-        <v>7473</v>
-      </c>
-      <c r="O6">
-        <v>7106</v>
-      </c>
-      <c r="P6">
+      <c r="N6" s="2">
+        <v>6978</v>
+      </c>
+      <c r="O6" s="2">
+        <v>6810</v>
+      </c>
+      <c r="P6" s="2">
         <f>0.000381057258287357*0.03</f>
         <v>1.143171774862071E-5</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="7" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
         <v>180</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="2">
         <v>25000</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="2">
         <v>71</v>
       </c>
-      <c r="D7">
-        <v>740</v>
-      </c>
-      <c r="E7">
-        <v>42767</v>
-      </c>
-      <c r="F7">
+      <c r="D7" s="2">
+        <v>613</v>
+      </c>
+      <c r="E7" s="2">
+        <v>39804</v>
+      </c>
+      <c r="F7" s="2">
         <v>604</v>
       </c>
-      <c r="G7">
-        <v>44182</v>
-      </c>
-      <c r="H7">
-        <v>55</v>
-      </c>
-      <c r="I7">
-        <v>190</v>
-      </c>
-      <c r="J7">
-        <v>33</v>
-      </c>
-      <c r="K7">
-        <v>15196</v>
-      </c>
-      <c r="L7">
-        <v>1535</v>
-      </c>
-      <c r="M7">
-        <v>495</v>
-      </c>
-      <c r="N7">
-        <v>17504</v>
-      </c>
-      <c r="O7">
-        <v>17259</v>
-      </c>
-      <c r="P7">
+      <c r="G7" s="2">
+        <v>41092</v>
+      </c>
+      <c r="H7" s="2">
+        <v>41</v>
+      </c>
+      <c r="I7" s="2">
+        <v>147</v>
+      </c>
+      <c r="J7" s="2">
+        <v>32</v>
+      </c>
+      <c r="K7" s="2">
+        <v>14295</v>
+      </c>
+      <c r="L7" s="2">
+        <v>1528</v>
+      </c>
+      <c r="M7" s="2">
+        <v>496</v>
+      </c>
+      <c r="N7" s="2">
+        <v>16539</v>
+      </c>
+      <c r="O7" s="2">
+        <v>16351</v>
+      </c>
+      <c r="P7" s="2">
         <f>0.000381057258287357*0.03</f>
         <v>1.143171774862071E-5</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9">
+    <row r="9" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
         <v>25</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="2">
         <v>640</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="2">
         <v>8</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="2">
         <v>11</v>
       </c>
-      <c r="E9">
-        <v>1354</v>
-      </c>
-      <c r="F9">
+      <c r="E9" s="2">
+        <v>1311</v>
+      </c>
+      <c r="F9" s="2">
         <v>19747</v>
       </c>
-      <c r="G9">
-        <v>21120</v>
-      </c>
-      <c r="H9">
-        <v>1</v>
-      </c>
-      <c r="I9">
-        <v>869</v>
-      </c>
-      <c r="J9">
+      <c r="G9" s="2">
+        <v>21077</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0</v>
+      </c>
+      <c r="I9" s="2">
+        <v>848</v>
+      </c>
+      <c r="J9" s="2">
         <v>10</v>
       </c>
-      <c r="K9">
-        <v>695</v>
-      </c>
-      <c r="L9">
-        <v>279</v>
-      </c>
-      <c r="M9">
-        <v>17263</v>
-      </c>
-      <c r="N9">
-        <v>19117</v>
-      </c>
-      <c r="O9">
-        <v>18247</v>
-      </c>
-      <c r="P9">
+      <c r="K9" s="2">
+        <v>687</v>
+      </c>
+      <c r="L9" s="2">
+        <v>273</v>
+      </c>
+      <c r="M9" s="2">
+        <v>17254</v>
+      </c>
+      <c r="N9" s="2">
+        <v>19072</v>
+      </c>
+      <c r="O9" s="2">
+        <v>18224</v>
+      </c>
+      <c r="P9" s="2">
         <f>0.000381057258287357*0.03</f>
         <v>1.143171774862071E-5</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10">
+    <row r="10" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
         <v>25</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="2">
         <v>1600</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="2">
         <v>12</v>
       </c>
-      <c r="D10">
-        <v>37</v>
-      </c>
-      <c r="E10">
-        <v>2847</v>
-      </c>
-      <c r="F10">
+      <c r="D10" s="2">
+        <v>28</v>
+      </c>
+      <c r="E10" s="2">
+        <v>2749</v>
+      </c>
+      <c r="F10" s="2">
         <v>19750</v>
       </c>
-      <c r="G10">
-        <v>22646</v>
-      </c>
-      <c r="H10">
-        <v>2</v>
-      </c>
-      <c r="I10">
-        <v>595</v>
-      </c>
-      <c r="J10">
+      <c r="G10" s="2">
+        <v>22539</v>
+      </c>
+      <c r="H10" s="2">
+        <v>1</v>
+      </c>
+      <c r="I10" s="2">
+        <v>573</v>
+      </c>
+      <c r="J10" s="2">
         <v>13</v>
       </c>
-      <c r="K10">
-        <v>1313</v>
-      </c>
-      <c r="L10">
-        <v>403</v>
-      </c>
-      <c r="M10">
-        <v>17046</v>
-      </c>
-      <c r="N10">
-        <v>19372</v>
-      </c>
-      <c r="O10">
-        <v>18775</v>
-      </c>
-      <c r="P10">
+      <c r="K10" s="2">
+        <v>1277</v>
+      </c>
+      <c r="L10" s="2">
+        <v>395</v>
+      </c>
+      <c r="M10" s="2">
+        <v>17044</v>
+      </c>
+      <c r="N10" s="2">
+        <v>19303</v>
+      </c>
+      <c r="O10" s="2">
+        <v>18729</v>
+      </c>
+      <c r="P10" s="2">
         <f>0.000381057258287357*0.03</f>
         <v>1.143171774862071E-5</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11">
+    <row r="11" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
         <v>25</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="2">
         <v>4000</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="2">
         <v>13</v>
       </c>
-      <c r="D11">
-        <v>120</v>
-      </c>
-      <c r="E11">
-        <v>6659</v>
-      </c>
-      <c r="F11">
-        <v>19901</v>
-      </c>
-      <c r="G11">
-        <v>26693</v>
-      </c>
-      <c r="H11">
-        <v>4</v>
-      </c>
-      <c r="I11">
-        <v>560</v>
-      </c>
-      <c r="J11">
-        <v>15</v>
-      </c>
-      <c r="K11">
-        <v>2350</v>
-      </c>
-      <c r="L11">
-        <v>662</v>
-      </c>
-      <c r="M11">
-        <v>16614</v>
-      </c>
-      <c r="N11">
-        <v>20205</v>
-      </c>
-      <c r="O11">
-        <v>19641</v>
-      </c>
-      <c r="P11">
+      <c r="D11" s="2">
+        <v>107</v>
+      </c>
+      <c r="E11" s="2">
+        <v>6421</v>
+      </c>
+      <c r="F11" s="2">
+        <v>19900</v>
+      </c>
+      <c r="G11" s="2">
+        <v>26441</v>
+      </c>
+      <c r="H11" s="2">
+        <v>3</v>
+      </c>
+      <c r="I11" s="2">
+        <v>543</v>
+      </c>
+      <c r="J11" s="2">
+        <v>17</v>
+      </c>
+      <c r="K11" s="2">
+        <v>2283</v>
+      </c>
+      <c r="L11" s="2">
+        <v>658</v>
+      </c>
+      <c r="M11" s="2">
+        <v>16606</v>
+      </c>
+      <c r="N11" s="2">
+        <v>20110</v>
+      </c>
+      <c r="O11" s="2">
+        <v>19564</v>
+      </c>
+      <c r="P11" s="2">
         <f>0.000381057258287357*0.03</f>
         <v>1.143171774862071E-5</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12">
+    <row r="12" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
         <v>25</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="2">
         <v>10000</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="2">
         <v>51</v>
       </c>
-      <c r="D12">
-        <v>333</v>
-      </c>
-      <c r="E12">
-        <v>17567</v>
-      </c>
-      <c r="F12">
-        <v>19671</v>
-      </c>
-      <c r="G12">
-        <v>37622</v>
-      </c>
-      <c r="H12">
-        <v>20</v>
-      </c>
-      <c r="I12">
-        <v>264</v>
-      </c>
-      <c r="J12">
-        <v>41</v>
-      </c>
-      <c r="K12">
-        <v>6037</v>
-      </c>
-      <c r="L12">
-        <v>1153</v>
-      </c>
-      <c r="M12">
-        <v>15814</v>
-      </c>
-      <c r="N12">
-        <v>23329</v>
-      </c>
-      <c r="O12">
-        <v>23045</v>
-      </c>
-      <c r="P12">
+      <c r="D12" s="2">
+        <v>296</v>
+      </c>
+      <c r="E12" s="2">
+        <v>16634</v>
+      </c>
+      <c r="F12" s="2">
+        <v>19670</v>
+      </c>
+      <c r="G12" s="2">
+        <v>36651</v>
+      </c>
+      <c r="H12" s="2">
+        <v>17</v>
+      </c>
+      <c r="I12" s="2">
+        <v>246</v>
+      </c>
+      <c r="J12" s="2">
+        <v>38</v>
+      </c>
+      <c r="K12" s="2">
+        <v>5764</v>
+      </c>
+      <c r="L12" s="2">
+        <v>1135</v>
+      </c>
+      <c r="M12" s="2">
+        <v>15808</v>
+      </c>
+      <c r="N12" s="2">
+        <v>23008</v>
+      </c>
+      <c r="O12" s="2">
+        <v>22745</v>
+      </c>
+      <c r="P12" s="2">
         <f>0.000381057258287357*0.03</f>
         <v>1.143171774862071E-5</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13">
+    <row r="13" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
         <v>25</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="2">
         <v>25000</v>
       </c>
-      <c r="C13">
-        <v>110</v>
-      </c>
-      <c r="D13">
-        <v>761</v>
-      </c>
-      <c r="E13">
-        <v>42746</v>
-      </c>
-      <c r="F13">
-        <v>19236</v>
-      </c>
-      <c r="G13">
-        <v>62853</v>
-      </c>
-      <c r="H13">
-        <v>62</v>
-      </c>
-      <c r="I13">
-        <v>240</v>
-      </c>
-      <c r="J13">
-        <v>93</v>
-      </c>
-      <c r="K13">
-        <v>15622</v>
-      </c>
-      <c r="L13">
-        <v>1845</v>
-      </c>
-      <c r="M13">
-        <v>14215</v>
-      </c>
-      <c r="N13">
-        <v>32077</v>
-      </c>
-      <c r="O13">
-        <v>31775</v>
-      </c>
-      <c r="P13">
+      <c r="C13" s="2">
+        <v>111</v>
+      </c>
+      <c r="D13" s="2">
+        <v>581</v>
+      </c>
+      <c r="E13" s="2">
+        <v>39872</v>
+      </c>
+      <c r="F13" s="2">
+        <v>19234</v>
+      </c>
+      <c r="G13" s="2">
+        <v>59798</v>
+      </c>
+      <c r="H13" s="2">
+        <v>66</v>
+      </c>
+      <c r="I13" s="2">
+        <v>216</v>
+      </c>
+      <c r="J13" s="2">
+        <v>92</v>
+      </c>
+      <c r="K13" s="2">
+        <v>14765</v>
+      </c>
+      <c r="L13" s="2">
+        <v>1831</v>
+      </c>
+      <c r="M13" s="2">
+        <v>14214</v>
+      </c>
+      <c r="N13" s="2">
+        <v>31184</v>
+      </c>
+      <c r="O13" s="2">
+        <v>30902</v>
+      </c>
+      <c r="P13" s="2">
         <f>0.000381057258287357*0.03</f>
         <v>1.143171774862071E-5</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15">
+    <row r="15" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
         <v>10</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="2">
         <v>640</v>
       </c>
-      <c r="C15">
-        <v>31</v>
-      </c>
-      <c r="D15">
-        <v>16</v>
-      </c>
-      <c r="E15">
-        <v>1349</v>
-      </c>
-      <c r="F15">
-        <v>47751</v>
-      </c>
-      <c r="G15">
-        <v>49147</v>
-      </c>
-      <c r="H15">
-        <v>2</v>
-      </c>
-      <c r="I15">
-        <v>1097</v>
-      </c>
-      <c r="J15">
-        <v>52</v>
-      </c>
-      <c r="K15">
-        <v>778</v>
-      </c>
-      <c r="L15">
-        <v>208</v>
-      </c>
-      <c r="M15">
-        <v>39896</v>
-      </c>
-      <c r="N15">
-        <v>42033</v>
-      </c>
-      <c r="O15">
-        <v>40934</v>
-      </c>
-      <c r="P15">
+      <c r="C15" s="2">
+        <v>48</v>
+      </c>
+      <c r="D15" s="2">
+        <v>12</v>
+      </c>
+      <c r="E15" s="2">
+        <v>1314</v>
+      </c>
+      <c r="F15" s="2">
+        <v>47590</v>
+      </c>
+      <c r="G15" s="2">
+        <v>48964</v>
+      </c>
+      <c r="H15" s="2">
+        <v>0</v>
+      </c>
+      <c r="I15" s="2">
+        <v>1112</v>
+      </c>
+      <c r="J15" s="2">
+        <v>62</v>
+      </c>
+      <c r="K15" s="2">
+        <v>783</v>
+      </c>
+      <c r="L15" s="2">
+        <v>174</v>
+      </c>
+      <c r="M15" s="2">
+        <v>39734</v>
+      </c>
+      <c r="N15" s="2">
+        <v>41865</v>
+      </c>
+      <c r="O15" s="2">
+        <v>40753</v>
+      </c>
+      <c r="P15" s="2">
         <f>0.000381057258287357*0.03</f>
         <v>1.143171774862071E-5</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16">
+    <row r="16" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
         <v>10</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="2">
         <v>1600</v>
       </c>
-      <c r="C16">
-        <v>67</v>
-      </c>
-      <c r="D16">
+      <c r="C16" s="2">
+        <v>69</v>
+      </c>
+      <c r="D16" s="2">
         <v>23</v>
       </c>
-      <c r="E16">
-        <v>2861</v>
-      </c>
-      <c r="F16">
-        <v>47651</v>
-      </c>
-      <c r="G16">
-        <v>50602</v>
-      </c>
-      <c r="H16">
-        <v>2</v>
-      </c>
-      <c r="I16">
-        <v>797</v>
-      </c>
-      <c r="J16">
-        <v>77</v>
-      </c>
-      <c r="K16">
-        <v>1469</v>
-      </c>
-      <c r="L16">
-        <v>336</v>
-      </c>
-      <c r="M16">
-        <v>39388</v>
-      </c>
-      <c r="N16">
-        <v>42069</v>
-      </c>
-      <c r="O16">
-        <v>41270</v>
-      </c>
-      <c r="P16">
+      <c r="E16" s="2">
+        <v>2752</v>
+      </c>
+      <c r="F16" s="2">
+        <v>47594</v>
+      </c>
+      <c r="G16" s="2">
+        <v>50438</v>
+      </c>
+      <c r="H16" s="2">
+        <v>0</v>
+      </c>
+      <c r="I16" s="2">
+        <v>941</v>
+      </c>
+      <c r="J16" s="2">
+        <v>93</v>
+      </c>
+      <c r="K16" s="2">
+        <v>1425</v>
+      </c>
+      <c r="L16" s="2">
+        <v>351</v>
+      </c>
+      <c r="M16" s="2">
+        <v>39332</v>
+      </c>
+      <c r="N16" s="2">
+        <v>42142</v>
+      </c>
+      <c r="O16" s="2">
+        <v>41201</v>
+      </c>
+      <c r="P16" s="2">
         <f>0.000381057258287357*0.03</f>
         <v>1.143171774862071E-5</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A17">
+    <row r="17" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
         <v>10</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="2">
         <v>4000</v>
       </c>
-      <c r="C17">
-        <v>166</v>
-      </c>
-      <c r="D17">
+      <c r="C17" s="2">
+        <v>148</v>
+      </c>
+      <c r="D17" s="2">
         <v>104</v>
       </c>
-      <c r="E17">
-        <v>6675</v>
-      </c>
-      <c r="F17">
-        <v>47395</v>
-      </c>
-      <c r="G17">
-        <v>54340</v>
-      </c>
-      <c r="H17">
-        <v>8</v>
-      </c>
-      <c r="I17">
-        <v>525</v>
-      </c>
-      <c r="J17">
-        <v>130</v>
-      </c>
-      <c r="K17">
-        <v>2720</v>
-      </c>
-      <c r="L17">
-        <v>636</v>
-      </c>
-      <c r="M17">
-        <v>38436</v>
-      </c>
-      <c r="N17">
-        <v>42455</v>
-      </c>
-      <c r="O17">
-        <v>41922</v>
-      </c>
-      <c r="P17">
+      <c r="E17" s="2">
+        <v>6414</v>
+      </c>
+      <c r="F17" s="2">
+        <v>47972</v>
+      </c>
+      <c r="G17" s="2">
+        <v>54638</v>
+      </c>
+      <c r="H17" s="2">
+        <v>11</v>
+      </c>
+      <c r="I17" s="2">
+        <v>645</v>
+      </c>
+      <c r="J17" s="2">
+        <v>151</v>
+      </c>
+      <c r="K17" s="2">
+        <v>2590</v>
+      </c>
+      <c r="L17" s="2">
+        <v>632</v>
+      </c>
+      <c r="M17" s="2">
+        <v>38779</v>
+      </c>
+      <c r="N17" s="2">
+        <v>42808</v>
+      </c>
+      <c r="O17" s="2">
+        <v>42152</v>
+      </c>
+      <c r="P17" s="2">
         <f>0.000381057258287357*0.03</f>
         <v>1.143171774862071E-5</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A18">
+    <row r="18" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
         <v>10</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="2">
         <v>10000</v>
       </c>
-      <c r="C18">
-        <v>321</v>
-      </c>
-      <c r="D18">
-        <v>267</v>
-      </c>
-      <c r="E18">
-        <v>17633</v>
-      </c>
-      <c r="F18">
-        <v>47248</v>
-      </c>
-      <c r="G18">
-        <v>65469</v>
-      </c>
-      <c r="H18">
-        <v>13</v>
-      </c>
-      <c r="I18">
-        <v>655</v>
-      </c>
-      <c r="J18">
-        <v>262</v>
-      </c>
-      <c r="K18">
-        <v>6718</v>
-      </c>
-      <c r="L18">
-        <v>1091</v>
-      </c>
-      <c r="M18">
-        <v>36948</v>
-      </c>
-      <c r="N18">
-        <v>45687</v>
-      </c>
-      <c r="O18">
-        <v>45019</v>
-      </c>
-      <c r="P18">
+      <c r="C18" s="2">
+        <v>334</v>
+      </c>
+      <c r="D18" s="2">
+        <v>245</v>
+      </c>
+      <c r="E18" s="2">
+        <v>16701</v>
+      </c>
+      <c r="F18" s="2">
+        <v>47567</v>
+      </c>
+      <c r="G18" s="2">
+        <v>64847</v>
+      </c>
+      <c r="H18" s="2">
+        <v>18</v>
+      </c>
+      <c r="I18" s="2">
+        <v>541</v>
+      </c>
+      <c r="J18" s="2">
+        <v>266</v>
+      </c>
+      <c r="K18" s="2">
+        <v>6222</v>
+      </c>
+      <c r="L18" s="2">
+        <v>1147</v>
+      </c>
+      <c r="M18" s="2">
+        <v>37080</v>
+      </c>
+      <c r="N18" s="2">
+        <v>45274</v>
+      </c>
+      <c r="O18" s="2">
+        <v>44715</v>
+      </c>
+      <c r="P18" s="2">
         <f>0.000381057258287357*0.03</f>
         <v>1.143171774862071E-5</v>
       </c>
     </row>
-    <row r="19" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="3">
+    <row r="19" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
         <v>10</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B19" s="2">
         <v>25000</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19" s="2">
         <v>695</v>
       </c>
-      <c r="D19" s="3">
+      <c r="D19" s="2">
         <v>515</v>
       </c>
-      <c r="E19" s="3">
+      <c r="E19" s="2">
         <v>39917</v>
       </c>
-      <c r="F19" s="3">
+      <c r="F19" s="2">
         <v>47055</v>
       </c>
-      <c r="G19" s="3">
+      <c r="G19" s="2">
         <v>88182</v>
       </c>
-      <c r="H19" s="3">
+      <c r="H19" s="2">
         <v>76</v>
       </c>
-      <c r="I19" s="3">
+      <c r="I19" s="2">
         <v>382</v>
       </c>
-      <c r="J19" s="3">
+      <c r="J19" s="2">
         <v>467</v>
       </c>
-      <c r="K19" s="3">
+      <c r="K19" s="2">
         <v>14442</v>
       </c>
-      <c r="L19" s="3">
+      <c r="L19" s="2">
         <v>913</v>
       </c>
-      <c r="M19" s="3">
+      <c r="M19" s="2">
         <v>29726</v>
       </c>
-      <c r="N19" s="3">
+      <c r="N19" s="2">
         <v>51341</v>
       </c>
-      <c r="O19" s="3">
+      <c r="O19" s="2">
         <v>50853</v>
       </c>
     </row>
-    <row r="21" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="3">
+    <row r="21" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
         <v>5</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B21" s="2">
         <v>640</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C21" s="2">
         <v>28</v>
       </c>
-      <c r="D21" s="3">
+      <c r="D21" s="2">
         <v>18</v>
       </c>
-      <c r="E21" s="3">
+      <c r="E21" s="2">
         <v>1310</v>
       </c>
-      <c r="F21" s="3">
+      <c r="F21" s="2">
         <v>67618</v>
       </c>
-      <c r="G21" s="3">
+      <c r="G21" s="2">
         <v>68974</v>
       </c>
-      <c r="H21" s="3">
+      <c r="H21" s="2">
         <v>0</v>
       </c>
-      <c r="I21" s="3">
+      <c r="I21" s="2">
         <v>1063</v>
       </c>
-      <c r="J21" s="3">
+      <c r="J21" s="2">
         <v>35</v>
       </c>
-      <c r="K21" s="3">
+      <c r="K21" s="2">
         <v>552</v>
       </c>
-      <c r="L21" s="3">
+      <c r="L21" s="2">
         <v>429</v>
       </c>
-      <c r="M21" s="3">
+      <c r="M21" s="2">
         <v>55958</v>
       </c>
-      <c r="N21" s="3">
+      <c r="N21" s="2">
         <v>58037</v>
       </c>
-      <c r="O21" s="3">
+      <c r="O21" s="2">
         <v>56974</v>
       </c>
     </row>
-    <row r="22" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="3">
+    <row r="22" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
         <v>5</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B22" s="2">
         <v>1600</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C22" s="2">
         <v>61</v>
       </c>
-      <c r="D22" s="3">
+      <c r="D22" s="2">
         <v>28</v>
       </c>
-      <c r="E22" s="3">
+      <c r="E22" s="2">
         <v>2749</v>
       </c>
-      <c r="F22" s="3">
+      <c r="F22" s="2">
         <v>67696</v>
       </c>
-      <c r="G22" s="3">
+      <c r="G22" s="2">
         <v>70534</v>
       </c>
-      <c r="H22" s="3">
+      <c r="H22" s="2">
         <v>2</v>
       </c>
-      <c r="I22" s="3">
+      <c r="I22" s="2">
         <v>907</v>
       </c>
-      <c r="J22" s="3">
+      <c r="J22" s="2">
         <v>89</v>
       </c>
-      <c r="K22" s="3">
+      <c r="K22" s="2">
         <v>1280</v>
       </c>
-      <c r="L22" s="3">
+      <c r="L22" s="2">
         <v>533</v>
       </c>
-      <c r="M22" s="3">
+      <c r="M22" s="2">
         <v>55683</v>
       </c>
-      <c r="N22" s="3">
+      <c r="N22" s="2">
         <v>58494</v>
       </c>
-      <c r="O22" s="3">
+      <c r="O22" s="2">
         <v>57585</v>
       </c>
     </row>
-    <row r="23" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="3">
+    <row r="23" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
         <v>5</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B23" s="2">
         <v>4000</v>
       </c>
-      <c r="C23" s="3">
+      <c r="C23" s="2">
         <v>138</v>
       </c>
-      <c r="D23" s="3">
+      <c r="D23" s="2">
         <v>83</v>
       </c>
-      <c r="E23" s="3">
+      <c r="E23" s="2">
         <v>6434</v>
       </c>
-      <c r="F23" s="3">
+      <c r="F23" s="2">
         <v>67310</v>
       </c>
-      <c r="G23" s="3">
+      <c r="G23" s="2">
         <v>73965</v>
       </c>
-      <c r="H23" s="3">
+      <c r="H23" s="2">
         <v>5</v>
       </c>
-      <c r="I23" s="3">
+      <c r="I23" s="2">
         <v>1389</v>
       </c>
-      <c r="J23" s="3">
+      <c r="J23" s="2">
         <v>156</v>
       </c>
-      <c r="K23" s="3">
+      <c r="K23" s="2">
         <v>2647</v>
       </c>
-      <c r="L23" s="3">
+      <c r="L23" s="2">
         <v>764</v>
       </c>
-      <c r="M23" s="3">
+      <c r="M23" s="2">
         <v>53889</v>
       </c>
-      <c r="N23" s="3">
+      <c r="N23" s="2">
         <v>58850</v>
       </c>
-      <c r="O23" s="3">
+      <c r="O23" s="2">
         <v>57456</v>
       </c>
     </row>
-    <row r="24" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="3">
+    <row r="24" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
         <v>5</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B24" s="2">
         <v>10000</v>
       </c>
-      <c r="C24" s="3">
+      <c r="C24" s="2">
         <v>225</v>
       </c>
-      <c r="D24" s="3">
+      <c r="D24" s="2">
         <v>267</v>
       </c>
-      <c r="E24" s="3">
+      <c r="E24" s="2">
         <v>16686</v>
       </c>
-      <c r="F24" s="3">
+      <c r="F24" s="2">
         <v>66949</v>
       </c>
-      <c r="G24" s="3">
+      <c r="G24" s="2">
         <v>84127</v>
       </c>
-      <c r="H24" s="3">
+      <c r="H24" s="2">
         <v>25</v>
       </c>
-      <c r="I24" s="3">
+      <c r="I24" s="2">
         <v>709</v>
       </c>
-      <c r="J24" s="3">
+      <c r="J24" s="2">
         <v>238</v>
       </c>
-      <c r="K24" s="3">
+      <c r="K24" s="2">
         <v>6525</v>
       </c>
-      <c r="L24" s="3">
+      <c r="L24" s="2">
         <v>1316</v>
       </c>
-      <c r="M24" s="3">
+      <c r="M24" s="2">
         <v>52124</v>
       </c>
-      <c r="N24" s="3">
+      <c r="N24" s="2">
         <v>60937</v>
       </c>
-      <c r="O24" s="3">
+      <c r="O24" s="2">
         <v>60203</v>
       </c>
     </row>
-    <row r="25" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="3">
+    <row r="25" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
         <v>5</v>
       </c>
-      <c r="B25" s="3">
+      <c r="B25" s="2">
         <v>25000</v>
       </c>
-      <c r="C25" s="3">
+      <c r="C25" s="2">
         <v>576</v>
       </c>
-      <c r="D25" s="3">
+      <c r="D25" s="2">
         <v>594</v>
       </c>
-      <c r="E25" s="3">
+      <c r="E25" s="2">
         <v>39812</v>
       </c>
-      <c r="F25" s="3">
+      <c r="F25" s="2">
         <v>66947</v>
       </c>
-      <c r="G25" s="3">
+      <c r="G25" s="2">
         <v>107929</v>
       </c>
-      <c r="H25" s="3">
+      <c r="H25" s="2">
         <v>47</v>
       </c>
-      <c r="I25" s="3">
+      <c r="I25" s="2">
         <v>556</v>
       </c>
-      <c r="J25" s="3">
+      <c r="J25" s="2">
         <v>412</v>
       </c>
-      <c r="K25" s="3">
+      <c r="K25" s="2">
         <v>13788</v>
       </c>
-      <c r="L25" s="3">
+      <c r="L25" s="2">
         <v>2287</v>
       </c>
-      <c r="M25" s="3">
+      <c r="M25" s="2">
         <v>48020</v>
       </c>
-      <c r="N25" s="3">
+      <c r="N25" s="2">
         <v>65110</v>
       </c>
-      <c r="O25" s="3">
+      <c r="O25" s="2">
         <v>64507</v>
       </c>
     </row>
-    <row r="27" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="3">
+    <row r="27" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
         <v>0</v>
       </c>
-      <c r="B27" s="3">
+      <c r="B27" s="2">
         <v>640</v>
       </c>
-      <c r="C27" s="3">
+      <c r="C27" s="2">
         <v>121</v>
       </c>
-      <c r="D27" s="3">
+      <c r="D27" s="2">
         <v>17</v>
       </c>
-      <c r="E27" s="3">
+      <c r="E27" s="2">
         <v>1309</v>
       </c>
-      <c r="F27" s="3">
+      <c r="F27" s="2">
         <v>350653</v>
       </c>
-      <c r="G27" s="3">
+      <c r="G27" s="2">
         <v>352100</v>
       </c>
-      <c r="H27" s="3">
+      <c r="H27" s="2">
         <v>5</v>
       </c>
-      <c r="I27" s="3">
+      <c r="I27" s="2">
         <v>5418</v>
       </c>
-      <c r="J27" s="3">
+      <c r="J27" s="2">
         <v>256</v>
       </c>
-      <c r="K27" s="3">
+      <c r="K27" s="2">
         <v>564</v>
       </c>
-      <c r="L27" s="3">
+      <c r="L27" s="2">
         <v>369</v>
       </c>
-      <c r="M27" s="3">
+      <c r="M27" s="2">
         <v>267518</v>
       </c>
-      <c r="N27" s="3">
+      <c r="N27" s="2">
         <v>274130</v>
       </c>
-      <c r="O27" s="3">
+      <c r="O27" s="2">
         <v>268707</v>
       </c>
     </row>
-    <row r="28" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="3">
+    <row r="28" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
         <v>0</v>
       </c>
-      <c r="B28" s="3">
+      <c r="B28" s="2">
         <v>1600</v>
       </c>
-      <c r="C28" s="3">
+      <c r="C28" s="2">
         <v>224</v>
       </c>
-      <c r="D28" s="3">
+      <c r="D28" s="2">
         <v>36</v>
       </c>
-      <c r="E28" s="3">
+      <c r="E28" s="2">
         <v>2741</v>
       </c>
-      <c r="F28" s="3">
+      <c r="F28" s="2">
         <v>350394</v>
       </c>
-      <c r="G28" s="3">
+      <c r="G28" s="2">
         <v>353395</v>
       </c>
-      <c r="H28" s="3">
+      <c r="H28" s="2">
         <v>8</v>
       </c>
-      <c r="I28" s="3">
+      <c r="I28" s="2">
         <v>5566</v>
       </c>
-      <c r="J28" s="3">
+      <c r="J28" s="2">
         <v>409</v>
       </c>
-      <c r="K28" s="3">
+      <c r="K28" s="2">
         <v>1186</v>
       </c>
-      <c r="L28" s="3">
+      <c r="L28" s="2">
         <v>567</v>
       </c>
-      <c r="M28" s="3">
+      <c r="M28" s="2">
         <v>263821</v>
       </c>
-      <c r="N28" s="3">
+      <c r="N28" s="2">
         <v>271557</v>
       </c>
-      <c r="O28" s="3">
+      <c r="O28" s="2">
         <v>265983</v>
       </c>
     </row>
-    <row r="29" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="3">
+    <row r="29" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
         <v>0</v>
       </c>
-      <c r="B29" s="3">
+      <c r="B29" s="2">
         <v>4000</v>
       </c>
-      <c r="C29" s="3">
+      <c r="C29" s="2">
         <v>535</v>
       </c>
-      <c r="D29" s="3">
+      <c r="D29" s="2">
         <v>93</v>
       </c>
-      <c r="E29" s="3">
+      <c r="E29" s="2">
         <v>6428</v>
       </c>
-      <c r="F29" s="3">
+      <c r="F29" s="2">
         <v>350990</v>
       </c>
-      <c r="G29" s="3">
+      <c r="G29" s="2">
         <v>358046</v>
       </c>
-      <c r="H29" s="3">
+      <c r="H29" s="2">
         <v>17</v>
       </c>
-      <c r="I29" s="3">
+      <c r="I29" s="2">
         <v>5673</v>
       </c>
-      <c r="J29" s="3">
+      <c r="J29" s="2">
         <v>601</v>
       </c>
-      <c r="K29" s="3">
+      <c r="K29" s="2">
         <v>2786</v>
       </c>
-      <c r="L29" s="3">
+      <c r="L29" s="2">
         <v>1059</v>
       </c>
-      <c r="M29" s="3">
+      <c r="M29" s="2">
         <v>258710</v>
       </c>
-      <c r="N29" s="3">
+      <c r="N29" s="2">
         <v>268846</v>
       </c>
-      <c r="O29" s="3">
+      <c r="O29" s="2">
         <v>263156</v>
       </c>
     </row>
-    <row r="30" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="3">
+    <row r="30" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
         <v>0</v>
       </c>
-      <c r="B30" s="3">
+      <c r="B30" s="2">
         <v>10000</v>
       </c>
-      <c r="C30" s="3">
+      <c r="C30" s="2">
         <v>1120</v>
       </c>
-      <c r="D30" s="3">
+      <c r="D30" s="2">
         <v>207</v>
       </c>
-      <c r="E30" s="3">
+      <c r="E30" s="2">
         <v>16743</v>
       </c>
-      <c r="F30" s="3">
+      <c r="F30" s="2">
         <v>350661</v>
       </c>
-      <c r="G30" s="3">
+      <c r="G30" s="2">
         <v>368731</v>
       </c>
-      <c r="H30" s="3">
+      <c r="H30" s="2">
         <v>60</v>
       </c>
-      <c r="I30" s="3">
+      <c r="I30" s="2">
         <v>5698</v>
       </c>
-      <c r="J30" s="3">
+      <c r="J30" s="2">
         <v>1111</v>
       </c>
-      <c r="K30" s="3">
+      <c r="K30" s="2">
         <v>6343</v>
       </c>
-      <c r="L30" s="3">
+      <c r="L30" s="2">
         <v>1871</v>
       </c>
-      <c r="M30" s="3">
+      <c r="M30" s="2">
         <v>247466</v>
       </c>
-      <c r="N30" s="3">
+      <c r="N30" s="2">
         <v>262549</v>
       </c>
-      <c r="O30" s="3">
+      <c r="O30" s="2">
         <v>256791</v>
       </c>
     </row>
-    <row r="31" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="3">
+    <row r="31" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
         <v>0</v>
       </c>
-      <c r="B31" s="3">
+      <c r="B31" s="2">
         <v>25000</v>
       </c>
-      <c r="C31" s="3">
+      <c r="C31" s="2">
         <v>2352</v>
       </c>
-      <c r="D31" s="3">
+      <c r="D31" s="2">
         <v>566</v>
       </c>
-      <c r="E31" s="3">
+      <c r="E31" s="2">
         <v>39852</v>
       </c>
-      <c r="F31" s="3">
+      <c r="F31" s="2">
         <v>348478</v>
       </c>
-      <c r="G31" s="3">
+      <c r="G31" s="2">
         <v>391248</v>
       </c>
-      <c r="H31" s="3">
+      <c r="H31" s="2">
         <v>121</v>
       </c>
-      <c r="I31" s="3">
+      <c r="I31" s="2">
         <v>5115</v>
       </c>
-      <c r="J31" s="3">
+      <c r="J31" s="2">
         <v>1749</v>
       </c>
-      <c r="K31" s="3">
+      <c r="K31" s="2">
         <v>12600</v>
       </c>
-      <c r="L31" s="3">
+      <c r="L31" s="2">
         <v>3033</v>
       </c>
-      <c r="M31" s="3">
+      <c r="M31" s="2">
         <v>222476</v>
       </c>
-      <c r="N31" s="3">
+      <c r="N31" s="2">
         <v>245094</v>
       </c>
-      <c r="O31" s="3">
+      <c r="O31" s="2">
         <v>239858</v>
       </c>
     </row>

</xml_diff>

<commit_message>
obs rounding with gum. Map plots for all ranges
</commit_message>
<xml_diff>
--- a/Output/25_observations.xlsx
+++ b/Output/25_observations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Master_Thesis\VS_Project\N_Body\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{974AF6D4-CC80-40B6-AE77-E4AFE1391FE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A327822-D0FC-4CA0-880E-BBE9412BE6F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-30828" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="46">
   <si>
     <t>Mass</t>
   </si>
@@ -155,9 +155,6 @@
     <t>CTN 0.5 - 0.08</t>
   </si>
   <si>
-    <t>Conf</t>
-  </si>
-  <si>
     <t>True Positive / Total Positive</t>
   </si>
   <si>
@@ -174,6 +171,9 @@
   </si>
   <si>
     <t>Abs error</t>
+  </si>
+  <si>
+    <t>Sign Stellen</t>
   </si>
 </sst>
 </file>
@@ -506,10 +506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6C7D530-1791-4814-8A4A-F65FDE59479A}">
-  <dimension ref="A1:AR52"/>
+  <dimension ref="A1:AR54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="AP37" sqref="AP37"/>
+      <selection activeCell="AQ2" sqref="AQ2:AQ26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -618,22 +618,31 @@
         <v>14</v>
       </c>
       <c r="AI1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ1" t="s">
         <v>41</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>42</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>43</v>
       </c>
-      <c r="AL1" t="s">
-        <v>44</v>
+      <c r="AN1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>42</v>
       </c>
       <c r="AQ1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AR1" t="s">
         <v>39</v>
-      </c>
-      <c r="AR1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:44" x14ac:dyDescent="0.25">
@@ -785,6 +794,22 @@
         <f>AVERAGE(extinction!AL2:AL11)</f>
         <v>0.9997555012224939</v>
       </c>
+      <c r="AN2">
+        <f>ROUNDUP(AI2,-INT(LOG(AI2))+(LEN(AN28)-LEN(SUBSTITUTE(AN28,"0",))+1)-1)</f>
+        <v>0.99983999999999995</v>
+      </c>
+      <c r="AO2">
+        <f t="shared" ref="AO2:AQ17" si="0">ROUNDUP(AJ2,-INT(LOG(AJ2))+(LEN(AO28)-LEN(SUBSTITUTE(AO28,"0",))+1)-1)</f>
+        <v>1</v>
+      </c>
+      <c r="AP2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AQ2">
+        <f t="shared" si="0"/>
+        <v>0.99975999999999998</v>
+      </c>
     </row>
     <row r="3" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -935,6 +960,22 @@
         <f>AVERAGE(extinction!AL12:AL21)</f>
         <v>0.99925348516627643</v>
       </c>
+      <c r="AN3">
+        <f t="shared" ref="AN3:AN26" si="1">ROUNDUP(AI3,-INT(LOG(AI3))+(LEN(AN29)-LEN(SUBSTITUTE(AN29,"0",))+1)-1)</f>
+        <v>0.99947999999999992</v>
+      </c>
+      <c r="AO3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AP3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AQ3">
+        <f t="shared" si="0"/>
+        <v>0.99925999999999993</v>
+      </c>
     </row>
     <row r="4" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -1085,6 +1126,22 @@
         <f>AVERAGE(extinction!AL22:AL31)</f>
         <v>0.99864067350446706</v>
       </c>
+      <c r="AN4">
+        <f t="shared" si="1"/>
+        <v>0.99905999999999995</v>
+      </c>
+      <c r="AO4">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AP4">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AQ4">
+        <f t="shared" si="0"/>
+        <v>0.99864999999999993</v>
+      </c>
     </row>
     <row r="5" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -1235,6 +1292,22 @@
         <f>AVERAGE(extinction!AL32:AL41)</f>
         <v>0.99811142379856432</v>
       </c>
+      <c r="AN5">
+        <f t="shared" si="1"/>
+        <v>0.99863999999999997</v>
+      </c>
+      <c r="AO5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AP5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AQ5">
+        <f t="shared" si="0"/>
+        <v>0.99812000000000001</v>
+      </c>
     </row>
     <row r="6" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -1385,6 +1458,22 @@
         <f>AVERAGE(extinction!AL42:AL51)</f>
         <v>0.99218717686402047</v>
       </c>
+      <c r="AN6">
+        <f t="shared" si="1"/>
+        <v>0.99363999999999997</v>
+      </c>
+      <c r="AO6">
+        <f t="shared" si="0"/>
+        <v>0.99961</v>
+      </c>
+      <c r="AP6">
+        <f t="shared" si="0"/>
+        <v>0.99680000000000002</v>
+      </c>
+      <c r="AQ6">
+        <f t="shared" si="0"/>
+        <v>0.99219999999999997</v>
+      </c>
     </row>
     <row r="7" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -1535,6 +1624,22 @@
         <f>AVERAGE(extinction!AL52:AL61)</f>
         <v>0.95340527226277949</v>
       </c>
+      <c r="AN7">
+        <f t="shared" si="1"/>
+        <v>0.96119999999999994</v>
+      </c>
+      <c r="AO7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AP7">
+        <f t="shared" si="0"/>
+        <v>0.96970000000000001</v>
+      </c>
+      <c r="AQ7">
+        <f t="shared" si="0"/>
+        <v>0.95399999999999996</v>
+      </c>
     </row>
     <row r="8" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -1685,6 +1790,22 @@
         <f>AVERAGE(extinction!AL62:AL71)</f>
         <v>0.96011339265421147</v>
       </c>
+      <c r="AN8">
+        <f t="shared" si="1"/>
+        <v>0.96589999999999998</v>
+      </c>
+      <c r="AO8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AP8">
+        <f t="shared" si="0"/>
+        <v>0.97329999999999994</v>
+      </c>
+      <c r="AQ8">
+        <f t="shared" si="0"/>
+        <v>0.96099999999999997</v>
+      </c>
     </row>
     <row r="9" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -1835,6 +1956,22 @@
         <f>AVERAGE(extinction!AL72:AL81)</f>
         <v>0.97160640400551446</v>
       </c>
+      <c r="AN9">
+        <f t="shared" si="1"/>
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="AO9">
+        <f t="shared" si="0"/>
+        <v>0.99939999999999996</v>
+      </c>
+      <c r="AP9">
+        <f t="shared" si="0"/>
+        <v>0.98170000000000002</v>
+      </c>
+      <c r="AQ9">
+        <f t="shared" si="0"/>
+        <v>0.97170000000000001</v>
+      </c>
     </row>
     <row r="10" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -1985,6 +2122,22 @@
         <f>AVERAGE(extinction!AL82:AL91)</f>
         <v>0.97693511043876335</v>
       </c>
+      <c r="AN10">
+        <f t="shared" si="1"/>
+        <v>0.98080000000000001</v>
+      </c>
+      <c r="AO10">
+        <f t="shared" si="0"/>
+        <v>0.99973999999999996</v>
+      </c>
+      <c r="AP10">
+        <f t="shared" si="0"/>
+        <v>0.98739999999999994</v>
+      </c>
+      <c r="AQ10">
+        <f t="shared" si="0"/>
+        <v>0.97699999999999998</v>
+      </c>
     </row>
     <row r="11" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -2135,6 +2288,22 @@
         <f>AVERAGE(extinction!AL92:AL101)</f>
         <v>0.98281082492591465</v>
       </c>
+      <c r="AN11">
+        <f t="shared" si="1"/>
+        <v>0.98550000000000004</v>
+      </c>
+      <c r="AO11">
+        <f t="shared" si="0"/>
+        <v>0.99988999999999995</v>
+      </c>
+      <c r="AP11">
+        <f t="shared" si="0"/>
+        <v>0.98970000000000002</v>
+      </c>
+      <c r="AQ11">
+        <f t="shared" si="0"/>
+        <v>0.9829</v>
+      </c>
     </row>
     <row r="12" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -2285,6 +2454,22 @@
         <f>AVERAGE(extinction!AL102:AL111)</f>
         <v>0.80873698568982166</v>
       </c>
+      <c r="AN12">
+        <f t="shared" si="1"/>
+        <v>0.85599999999999998</v>
+      </c>
+      <c r="AO12">
+        <f t="shared" si="0"/>
+        <v>0.99199999999999999</v>
+      </c>
+      <c r="AP12">
+        <f t="shared" si="0"/>
+        <v>0.91400000000000003</v>
+      </c>
+      <c r="AQ12">
+        <f t="shared" si="0"/>
+        <v>0.80900000000000005</v>
+      </c>
     </row>
     <row r="13" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -2435,6 +2620,22 @@
         <f>AVERAGE(extinction!AL112:AL121)</f>
         <v>0.84692070302950806</v>
       </c>
+      <c r="AN13">
+        <f t="shared" si="1"/>
+        <v>0.87339999999999995</v>
+      </c>
+      <c r="AO13">
+        <f t="shared" si="0"/>
+        <v>0.99509999999999998</v>
+      </c>
+      <c r="AP13">
+        <f t="shared" si="0"/>
+        <v>0.90500000000000003</v>
+      </c>
+      <c r="AQ13">
+        <f t="shared" si="0"/>
+        <v>0.84699999999999998</v>
+      </c>
     </row>
     <row r="14" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -2585,6 +2786,22 @@
         <f>AVERAGE(extinction!AL122:AL131)</f>
         <v>0.87896264467508656</v>
       </c>
+      <c r="AN14">
+        <f t="shared" si="1"/>
+        <v>0.90159999999999996</v>
+      </c>
+      <c r="AO14">
+        <f t="shared" si="0"/>
+        <v>0.99749999999999994</v>
+      </c>
+      <c r="AP14">
+        <f t="shared" si="0"/>
+        <v>0.93300000000000005</v>
+      </c>
+      <c r="AQ14">
+        <f t="shared" si="0"/>
+        <v>0.879</v>
+      </c>
     </row>
     <row r="15" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A15">
@@ -2735,6 +2952,22 @@
         <f>AVERAGE(extinction!AL132:AL141)</f>
         <v>0.91674961571996794</v>
       </c>
+      <c r="AN15">
+        <f t="shared" si="1"/>
+        <v>0.92999999999999994</v>
+      </c>
+      <c r="AO15">
+        <f t="shared" si="0"/>
+        <v>0.99809999999999999</v>
+      </c>
+      <c r="AP15">
+        <f t="shared" si="0"/>
+        <v>0.94840000000000002</v>
+      </c>
+      <c r="AQ15">
+        <f t="shared" si="0"/>
+        <v>0.91679999999999995</v>
+      </c>
     </row>
     <row r="16" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A16">
@@ -2885,8 +3118,24 @@
         <f>AVERAGE(extinction!AL142:AL151)</f>
         <v>0.94221837094486016</v>
       </c>
+      <c r="AN16">
+        <f t="shared" si="1"/>
+        <v>0.95069999999999999</v>
+      </c>
+      <c r="AO16">
+        <f t="shared" si="0"/>
+        <v>0.99819999999999998</v>
+      </c>
+      <c r="AP16">
+        <f t="shared" si="0"/>
+        <v>0.96160000000000001</v>
+      </c>
+      <c r="AQ16">
+        <f t="shared" si="0"/>
+        <v>0.94230000000000003</v>
+      </c>
     </row>
-    <row r="17" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A17">
         <f>AVERAGE(extinction!A152:A161)</f>
         <v>5</v>
@@ -3035,8 +3284,24 @@
         <f>AVERAGE(extinction!AL152:AL161)</f>
         <v>0.87092979629907852</v>
       </c>
+      <c r="AN17">
+        <f t="shared" si="1"/>
+        <v>0.92700000000000005</v>
+      </c>
+      <c r="AO17">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AP17">
+        <f t="shared" si="0"/>
+        <v>0.96829999999999994</v>
+      </c>
+      <c r="AQ17">
+        <f t="shared" si="0"/>
+        <v>0.871</v>
+      </c>
     </row>
-    <row r="18" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A18">
         <f>AVERAGE(extinction!A162:A171)</f>
         <v>5</v>
@@ -3185,8 +3450,24 @@
         <f>AVERAGE(extinction!AL162:AL171)</f>
         <v>0.91248506851226363</v>
       </c>
+      <c r="AN18">
+        <f t="shared" si="1"/>
+        <v>0.93959999999999999</v>
+      </c>
+      <c r="AO18">
+        <f t="shared" ref="AO18:AO26" si="2">ROUNDUP(AJ18,-INT(LOG(AJ18))+(LEN(AO44)-LEN(SUBSTITUTE(AO44,"0",))+1)-1)</f>
+        <v>0.99870000000000003</v>
+      </c>
+      <c r="AP18">
+        <f t="shared" ref="AP18:AP26" si="3">ROUNDUP(AK18,-INT(LOG(AK18))+(LEN(AP44)-LEN(SUBSTITUTE(AP44,"0",))+1)-1)</f>
+        <v>0.96850000000000003</v>
+      </c>
+      <c r="AQ18">
+        <f t="shared" ref="AQ18:AQ26" si="4">ROUNDUP(AL18,-INT(LOG(AL18))+(LEN(AQ44)-LEN(SUBSTITUTE(AQ44,"0",))+1)-1)</f>
+        <v>0.91300000000000003</v>
+      </c>
     </row>
-    <row r="19" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A19">
         <f>AVERAGE(extinction!A172:A181)</f>
         <v>5</v>
@@ -3335,8 +3616,24 @@
         <f>AVERAGE(extinction!AL172:AL181)</f>
         <v>0.93840802569631188</v>
       </c>
+      <c r="AN19">
+        <f t="shared" si="1"/>
+        <v>0.95669999999999999</v>
+      </c>
+      <c r="AO19">
+        <f t="shared" si="2"/>
+        <v>0.99849999999999994</v>
+      </c>
+      <c r="AP19">
+        <f t="shared" si="3"/>
+        <v>0.97799999999999998</v>
+      </c>
+      <c r="AQ19">
+        <f t="shared" si="4"/>
+        <v>0.9385</v>
+      </c>
     </row>
-    <row r="20" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A20">
         <f>AVERAGE(extinction!A182:A191)</f>
         <v>5</v>
@@ -3485,8 +3782,24 @@
         <f>AVERAGE(extinction!AL182:AL191)</f>
         <v>0.95184777080486982</v>
       </c>
+      <c r="AN20">
+        <f t="shared" si="1"/>
+        <v>0.96319999999999995</v>
+      </c>
+      <c r="AO20">
+        <f t="shared" si="2"/>
+        <v>0.99909999999999999</v>
+      </c>
+      <c r="AP20">
+        <f t="shared" si="3"/>
+        <v>0.97889999999999999</v>
+      </c>
+      <c r="AQ20">
+        <f t="shared" si="4"/>
+        <v>0.95189999999999997</v>
+      </c>
     </row>
-    <row r="21" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A21">
         <f>AVERAGE(extinction!A192:A201)</f>
         <v>5</v>
@@ -3635,8 +3948,24 @@
         <f>AVERAGE(extinction!AL192:AL201)</f>
         <v>0.96418226389131756</v>
       </c>
+      <c r="AN21">
+        <f t="shared" si="1"/>
+        <v>0.97260000000000002</v>
+      </c>
+      <c r="AO21">
+        <f t="shared" si="2"/>
+        <v>0.99929999999999997</v>
+      </c>
+      <c r="AP21">
+        <f t="shared" si="3"/>
+        <v>0.9839</v>
+      </c>
+      <c r="AQ21">
+        <f t="shared" si="4"/>
+        <v>0.96419999999999995</v>
+      </c>
     </row>
-    <row r="22" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A22">
         <f>AVERAGE(extinction!A202:A211)</f>
         <v>0</v>
@@ -3785,8 +4114,24 @@
         <f>AVERAGE(extinction!AL202:AL211)</f>
         <v>0.48650539393103187</v>
       </c>
+      <c r="AN22">
+        <f t="shared" si="1"/>
+        <v>0.626</v>
+      </c>
+      <c r="AO22">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AP22">
+        <f t="shared" si="3"/>
+        <v>0.80900000000000005</v>
+      </c>
+      <c r="AQ22">
+        <f t="shared" si="4"/>
+        <v>0.48699999999999999</v>
+      </c>
     </row>
-    <row r="23" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A23">
         <f>AVERAGE(extinction!A212:A221)</f>
         <v>0</v>
@@ -3935,8 +4280,24 @@
         <f>AVERAGE(extinction!AL212:AL221)</f>
         <v>0.61211959542307492</v>
       </c>
+      <c r="AN23">
+        <f t="shared" si="1"/>
+        <v>0.69799999999999995</v>
+      </c>
+      <c r="AO23">
+        <f t="shared" si="2"/>
+        <v>0.99760000000000004</v>
+      </c>
+      <c r="AP23">
+        <f t="shared" si="3"/>
+        <v>0.81699999999999995</v>
+      </c>
+      <c r="AQ23">
+        <f t="shared" si="4"/>
+        <v>0.61299999999999999</v>
+      </c>
     </row>
-    <row r="24" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A24">
         <f>AVERAGE(extinction!A222:A231)</f>
         <v>0</v>
@@ -4085,8 +4446,24 @@
         <f>AVERAGE(extinction!AL222:AL231)</f>
         <v>0.69849066224978862</v>
       </c>
+      <c r="AN24">
+        <f t="shared" si="1"/>
+        <v>0.77129999999999999</v>
+      </c>
+      <c r="AO24">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AP24">
+        <f t="shared" si="3"/>
+        <v>0.87219999999999998</v>
+      </c>
+      <c r="AQ24">
+        <f t="shared" si="4"/>
+        <v>0.69850000000000001</v>
+      </c>
     </row>
-    <row r="25" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A25">
         <f>AVERAGE(extinction!A232:A241)</f>
         <v>0</v>
@@ -4235,8 +4612,24 @@
         <f>AVERAGE(extinction!AL232:AL241)</f>
         <v>0.77185026390474121</v>
       </c>
+      <c r="AN25">
+        <f t="shared" si="1"/>
+        <v>0.82369999999999999</v>
+      </c>
+      <c r="AO25">
+        <f t="shared" si="2"/>
+        <v>0.99960000000000004</v>
+      </c>
+      <c r="AP25">
+        <f t="shared" si="3"/>
+        <v>0.89900000000000002</v>
+      </c>
+      <c r="AQ25">
+        <f t="shared" si="4"/>
+        <v>0.77190000000000003</v>
+      </c>
     </row>
-    <row r="26" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A26">
         <f>AVERAGE(extinction!A242:A251)</f>
         <v>0</v>
@@ -4385,13 +4778,29 @@
         <f>AVERAGE(extinction!AL242:AL251)</f>
         <v>0.82119188664169729</v>
       </c>
+      <c r="AN26">
+        <f t="shared" si="1"/>
+        <v>0.86660000000000004</v>
+      </c>
+      <c r="AO26">
+        <f t="shared" si="2"/>
+        <v>0.9996799999999999</v>
+      </c>
+      <c r="AP26">
+        <f t="shared" si="3"/>
+        <v>0.92610000000000003</v>
+      </c>
+      <c r="AQ26">
+        <f t="shared" si="4"/>
+        <v>0.82120000000000004</v>
+      </c>
     </row>
-    <row r="27" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:43" x14ac:dyDescent="0.25">
       <c r="O27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
-    <row r="28" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A28">
         <f>_xlfn.STDEV.S(extinction!A2:A11)</f>
         <v>0</v>
@@ -4540,8 +4949,24 @@
         <f>_xlfn.STDEV.S(extinction!AL2:AL11)</f>
         <v>7.7317302204604461E-4</v>
       </c>
+      <c r="AN28">
+        <f>IFERROR(ROUNDUP(AI28,-INT(LOG(AI28))+($AO$54-1)),0)</f>
+        <v>5.4000000000000001E-4</v>
+      </c>
+      <c r="AO28">
+        <f>IFERROR(ROUNDUP(AJ28,-INT(LOG(AJ28))+($AO$54-1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AP28">
+        <f>IFERROR(ROUNDUP(AK28,-INT(LOG(AK28))+($AO$54-1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AQ28">
+        <f>IFERROR(ROUNDUP(AL28,-INT(LOG(AL28))+($AO$54-1)),0)</f>
+        <v>7.7999999999999999E-4</v>
+      </c>
     </row>
-    <row r="29" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A29">
         <f>_xlfn.STDEV.S(extinction!A12:A21)</f>
         <v>0</v>
@@ -4690,8 +5115,24 @@
         <f>_xlfn.STDEV.S(extinction!AL12:AL21)</f>
         <v>8.705045734712641E-4</v>
       </c>
+      <c r="AN29">
+        <f>IFERROR(ROUNDUP(AI29,-INT(LOG(AI29))+($AO$54-1)),0)</f>
+        <v>6.2E-4</v>
+      </c>
+      <c r="AO29">
+        <f>IFERROR(ROUNDUP(AJ29,-INT(LOG(AJ29))+($AO$54-1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AP29">
+        <f>IFERROR(ROUNDUP(AK29,-INT(LOG(AK29))+($AO$54-1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AQ29">
+        <f>IFERROR(ROUNDUP(AL29,-INT(LOG(AL29))+($AO$54-1)),0)</f>
+        <v>8.8000000000000003E-4</v>
+      </c>
     </row>
-    <row r="30" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A30">
         <f>_xlfn.STDEV.S(extinction!A22:A31)</f>
         <v>0</v>
@@ -4840,8 +5281,24 @@
         <f>_xlfn.STDEV.S(extinction!AL22:AL31)</f>
         <v>7.7960709217457362E-4</v>
       </c>
+      <c r="AN30">
+        <f>IFERROR(ROUNDUP(AI30,-INT(LOG(AI30))+($AO$54-1)),0)</f>
+        <v>5.5000000000000003E-4</v>
+      </c>
+      <c r="AO30">
+        <f>IFERROR(ROUNDUP(AJ30,-INT(LOG(AJ30))+($AO$54-1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AP30">
+        <f>IFERROR(ROUNDUP(AK30,-INT(LOG(AK30))+($AO$54-1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AQ30">
+        <f>IFERROR(ROUNDUP(AL30,-INT(LOG(AL30))+($AO$54-1)),0)</f>
+        <v>7.7999999999999999E-4</v>
+      </c>
     </row>
-    <row r="31" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A31">
         <f>_xlfn.STDEV.S(extinction!A32:A41)</f>
         <v>0</v>
@@ -4990,8 +5447,24 @@
         <f>_xlfn.STDEV.S(extinction!AL32:AL41)</f>
         <v>7.1754529511924858E-4</v>
       </c>
+      <c r="AN31">
+        <f>IFERROR(ROUNDUP(AI31,-INT(LOG(AI31))+($AO$54-1)),0)</f>
+        <v>5.2000000000000006E-4</v>
+      </c>
+      <c r="AO31">
+        <f>IFERROR(ROUNDUP(AJ31,-INT(LOG(AJ31))+($AO$54-1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AP31">
+        <f>IFERROR(ROUNDUP(AK31,-INT(LOG(AK31))+($AO$54-1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AQ31">
+        <f>IFERROR(ROUNDUP(AL31,-INT(LOG(AL31))+($AO$54-1)),0)</f>
+        <v>7.2000000000000005E-4</v>
+      </c>
     </row>
-    <row r="32" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A32">
         <f>_xlfn.STDEV.S(extinction!A42:A51)</f>
         <v>0</v>
@@ -5140,8 +5613,24 @@
         <f>_xlfn.STDEV.S(extinction!AL42:AL51)</f>
         <v>1.2801559329646821E-3</v>
       </c>
+      <c r="AN32">
+        <f>IFERROR(ROUNDUP(AI32,-INT(LOG(AI32))+($AO$54-1)),0)</f>
+        <v>9.6000000000000002E-4</v>
+      </c>
+      <c r="AO32">
+        <f>IFERROR(ROUNDUP(AJ32,-INT(LOG(AJ32))+($AO$54-1)),0)</f>
+        <v>8.9000000000000006E-4</v>
+      </c>
+      <c r="AP32">
+        <f>IFERROR(ROUNDUP(AK32,-INT(LOG(AK32))+($AO$54-1)),0)</f>
+        <v>1.1000000000000001E-3</v>
+      </c>
+      <c r="AQ32">
+        <f>IFERROR(ROUNDUP(AL32,-INT(LOG(AL32))+($AO$54-1)),0)</f>
+        <v>1.2999999999999999E-3</v>
+      </c>
     </row>
-    <row r="33" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A33">
         <f>_xlfn.STDEV.S(extinction!A52:A61)</f>
         <v>0</v>
@@ -5290,8 +5779,24 @@
         <f>_xlfn.STDEV.S(extinction!AL52:AL61)</f>
         <v>1.3645766534354793E-2</v>
       </c>
+      <c r="AN33">
+        <f>IFERROR(ROUNDUP(AI33,-INT(LOG(AI33))+($AO$54-1)),0)</f>
+        <v>8.199999999999999E-3</v>
+      </c>
+      <c r="AO33">
+        <f>IFERROR(ROUNDUP(AJ33,-INT(LOG(AJ33))+($AO$54-1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AP33">
+        <f>IFERROR(ROUNDUP(AK33,-INT(LOG(AK33))+($AO$54-1)),0)</f>
+        <v>8.7999999999999988E-3</v>
+      </c>
+      <c r="AQ33">
+        <f>IFERROR(ROUNDUP(AL33,-INT(LOG(AL33))+($AO$54-1)),0)</f>
+        <v>1.3999999999999999E-2</v>
+      </c>
     </row>
-    <row r="34" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A34">
         <f>_xlfn.STDEV.S(extinction!A62:A71)</f>
         <v>0</v>
@@ -5440,8 +5945,24 @@
         <f>_xlfn.STDEV.S(extinction!AL62:AL71)</f>
         <v>1.0659774809532712E-2</v>
       </c>
+      <c r="AN34">
+        <f>IFERROR(ROUNDUP(AI34,-INT(LOG(AI34))+($AO$54-1)),0)</f>
+        <v>7.7000000000000002E-3</v>
+      </c>
+      <c r="AO34">
+        <f>IFERROR(ROUNDUP(AJ34,-INT(LOG(AJ34))+($AO$54-1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AP34">
+        <f>IFERROR(ROUNDUP(AK34,-INT(LOG(AK34))+($AO$54-1)),0)</f>
+        <v>8.3000000000000001E-3</v>
+      </c>
+      <c r="AQ34">
+        <f>IFERROR(ROUNDUP(AL34,-INT(LOG(AL34))+($AO$54-1)),0)</f>
+        <v>1.0999999999999999E-2</v>
+      </c>
     </row>
-    <row r="35" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A35">
         <f>_xlfn.STDEV.S(extinction!A72:A81)</f>
         <v>0</v>
@@ -5590,8 +6111,24 @@
         <f>_xlfn.STDEV.S(extinction!AL72:AL81)</f>
         <v>4.1662772644016173E-3</v>
       </c>
+      <c r="AN35">
+        <f>IFERROR(ROUNDUP(AI35,-INT(LOG(AI35))+($AO$54-1)),0)</f>
+        <v>3.5999999999999999E-3</v>
+      </c>
+      <c r="AO35">
+        <f>IFERROR(ROUNDUP(AJ35,-INT(LOG(AJ35))+($AO$54-1)),0)</f>
+        <v>2E-3</v>
+      </c>
+      <c r="AP35">
+        <f>IFERROR(ROUNDUP(AK35,-INT(LOG(AK35))+($AO$54-1)),0)</f>
+        <v>5.2000000000000006E-3</v>
+      </c>
+      <c r="AQ35">
+        <f>IFERROR(ROUNDUP(AL35,-INT(LOG(AL35))+($AO$54-1)),0)</f>
+        <v>4.2000000000000006E-3</v>
+      </c>
     </row>
-    <row r="36" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A36">
         <f>_xlfn.STDEV.S(extinction!A82:A91)</f>
         <v>0</v>
@@ -5740,8 +6277,24 @@
         <f>_xlfn.STDEV.S(extinction!AL82:AL91)</f>
         <v>1.5215975622081255E-3</v>
       </c>
+      <c r="AN36">
+        <f>IFERROR(ROUNDUP(AI36,-INT(LOG(AI36))+($AO$54-1)),0)</f>
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="AO36">
+        <f>IFERROR(ROUNDUP(AJ36,-INT(LOG(AJ36))+($AO$54-1)),0)</f>
+        <v>8.5999999999999998E-4</v>
+      </c>
+      <c r="AP36">
+        <f>IFERROR(ROUNDUP(AK36,-INT(LOG(AK36))+($AO$54-1)),0)</f>
+        <v>4.1000000000000003E-3</v>
+      </c>
+      <c r="AQ36">
+        <f>IFERROR(ROUNDUP(AL36,-INT(LOG(AL36))+($AO$54-1)),0)</f>
+        <v>1.6000000000000001E-3</v>
+      </c>
     </row>
-    <row r="37" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A37">
         <f>_xlfn.STDEV.S(extinction!A92:A101)</f>
         <v>0</v>
@@ -5890,8 +6443,24 @@
         <f>_xlfn.STDEV.S(extinction!AL92:AL101)</f>
         <v>1.5656771834241798E-3</v>
       </c>
+      <c r="AN37">
+        <f>IFERROR(ROUNDUP(AI37,-INT(LOG(AI37))+($AO$54-1)),0)</f>
+        <v>1.2000000000000001E-3</v>
+      </c>
+      <c r="AO37">
+        <f>IFERROR(ROUNDUP(AJ37,-INT(LOG(AJ37))+($AO$54-1)),0)</f>
+        <v>3.8000000000000002E-4</v>
+      </c>
+      <c r="AP37">
+        <f>IFERROR(ROUNDUP(AK37,-INT(LOG(AK37))+($AO$54-1)),0)</f>
+        <v>1.2000000000000001E-3</v>
+      </c>
+      <c r="AQ37">
+        <f>IFERROR(ROUNDUP(AL37,-INT(LOG(AL37))+($AO$54-1)),0)</f>
+        <v>1.6000000000000001E-3</v>
+      </c>
     </row>
-    <row r="38" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A38">
         <f>_xlfn.STDEV.S(extinction!A102:A111)</f>
         <v>0</v>
@@ -6040,8 +6609,24 @@
         <f>_xlfn.STDEV.S(extinction!AL102:AL111)</f>
         <v>2.1513200275154867E-2</v>
       </c>
+      <c r="AN38">
+        <f>IFERROR(ROUNDUP(AI38,-INT(LOG(AI38))+($AO$54-1)),0)</f>
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="AO38">
+        <f>IFERROR(ROUNDUP(AJ38,-INT(LOG(AJ38))+($AO$54-1)),0)</f>
+        <v>1.9E-2</v>
+      </c>
+      <c r="AP38">
+        <f>IFERROR(ROUNDUP(AK38,-INT(LOG(AK38))+($AO$54-1)),0)</f>
+        <v>1.8000000000000002E-2</v>
+      </c>
+      <c r="AQ38">
+        <f>IFERROR(ROUNDUP(AL38,-INT(LOG(AL38))+($AO$54-1)),0)</f>
+        <v>2.2000000000000002E-2</v>
+      </c>
     </row>
-    <row r="39" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A39">
         <f>_xlfn.STDEV.S(extinction!A112:A121)</f>
         <v>0</v>
@@ -6190,8 +6775,24 @@
         <f>_xlfn.STDEV.S(extinction!AL112:AL121)</f>
         <v>8.2640831017031947E-3</v>
       </c>
+      <c r="AN39">
+        <f>IFERROR(ROUNDUP(AI39,-INT(LOG(AI39))+($AO$54-1)),0)</f>
+        <v>7.2000000000000007E-3</v>
+      </c>
+      <c r="AO39">
+        <f>IFERROR(ROUNDUP(AJ39,-INT(LOG(AJ39))+($AO$54-1)),0)</f>
+        <v>8.8999999999999999E-3</v>
+      </c>
+      <c r="AP39">
+        <f>IFERROR(ROUNDUP(AK39,-INT(LOG(AK39))+($AO$54-1)),0)</f>
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="AQ39">
+        <f>IFERROR(ROUNDUP(AL39,-INT(LOG(AL39))+($AO$54-1)),0)</f>
+        <v>8.3000000000000001E-3</v>
+      </c>
     </row>
-    <row r="40" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A40">
         <f>_xlfn.STDEV.S(extinction!A122:A131)</f>
         <v>0</v>
@@ -6340,8 +6941,24 @@
         <f>_xlfn.STDEV.S(extinction!AL122:AL131)</f>
         <v>7.9550703392350149E-3</v>
       </c>
+      <c r="AN40">
+        <f>IFERROR(ROUNDUP(AI40,-INT(LOG(AI40))+($AO$54-1)),0)</f>
+        <v>8.199999999999999E-3</v>
+      </c>
+      <c r="AO40">
+        <f>IFERROR(ROUNDUP(AJ40,-INT(LOG(AJ40))+($AO$54-1)),0)</f>
+        <v>2.6999999999999997E-3</v>
+      </c>
+      <c r="AP40">
+        <f>IFERROR(ROUNDUP(AK40,-INT(LOG(AK40))+($AO$54-1)),0)</f>
+        <v>1.2E-2</v>
+      </c>
+      <c r="AQ40">
+        <f>IFERROR(ROUNDUP(AL40,-INT(LOG(AL40))+($AO$54-1)),0)</f>
+        <v>8.0000000000000002E-3</v>
+      </c>
     </row>
-    <row r="41" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A41">
         <f>_xlfn.STDEV.S(extinction!A132:A141)</f>
         <v>0</v>
@@ -6490,8 +7107,24 @@
         <f>_xlfn.STDEV.S(extinction!AL132:AL141)</f>
         <v>1.6056875973147939E-3</v>
       </c>
+      <c r="AN41">
+        <f>IFERROR(ROUNDUP(AI41,-INT(LOG(AI41))+($AO$54-1)),0)</f>
+        <v>2E-3</v>
+      </c>
+      <c r="AO41">
+        <f>IFERROR(ROUNDUP(AJ41,-INT(LOG(AJ41))+($AO$54-1)),0)</f>
+        <v>1.1000000000000001E-3</v>
+      </c>
+      <c r="AP41">
+        <f>IFERROR(ROUNDUP(AK41,-INT(LOG(AK41))+($AO$54-1)),0)</f>
+        <v>6.2000000000000006E-3</v>
+      </c>
+      <c r="AQ41">
+        <f>IFERROR(ROUNDUP(AL41,-INT(LOG(AL41))+($AO$54-1)),0)</f>
+        <v>1.7000000000000001E-3</v>
+      </c>
     </row>
-    <row r="42" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A42">
         <f>_xlfn.STDEV.S(extinction!A142:A151)</f>
         <v>0</v>
@@ -6640,8 +7273,24 @@
         <f>_xlfn.STDEV.S(extinction!AL142:AL151)</f>
         <v>2.3677574701317745E-3</v>
       </c>
+      <c r="AN42">
+        <f>IFERROR(ROUNDUP(AI42,-INT(LOG(AI42))+($AO$54-1)),0)</f>
+        <v>2.1999999999999997E-3</v>
+      </c>
+      <c r="AO42">
+        <f>IFERROR(ROUNDUP(AJ42,-INT(LOG(AJ42))+($AO$54-1)),0)</f>
+        <v>1.9E-3</v>
+      </c>
+      <c r="AP42">
+        <f>IFERROR(ROUNDUP(AK42,-INT(LOG(AK42))+($AO$54-1)),0)</f>
+        <v>4.4000000000000003E-3</v>
+      </c>
+      <c r="AQ42">
+        <f>IFERROR(ROUNDUP(AL42,-INT(LOG(AL42))+($AO$54-1)),0)</f>
+        <v>2.3999999999999998E-3</v>
+      </c>
     </row>
-    <row r="43" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A43">
         <f>_xlfn.STDEV.S(extinction!A152:A161)</f>
         <v>0</v>
@@ -6790,8 +7439,24 @@
         <f>_xlfn.STDEV.S(extinction!AL152:AL161)</f>
         <v>2.829875341561092E-2</v>
       </c>
+      <c r="AN43">
+        <f>IFERROR(ROUNDUP(AI43,-INT(LOG(AI43))+($AO$54-1)),0)</f>
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="AO43">
+        <f>IFERROR(ROUNDUP(AJ43,-INT(LOG(AJ43))+($AO$54-1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AP43">
+        <f>IFERROR(ROUNDUP(AK43,-INT(LOG(AK43))+($AO$54-1)),0)</f>
+        <v>8.6999999999999994E-3</v>
+      </c>
+      <c r="AQ43">
+        <f>IFERROR(ROUNDUP(AL43,-INT(LOG(AL43))+($AO$54-1)),0)</f>
+        <v>2.9000000000000001E-2</v>
+      </c>
     </row>
-    <row r="44" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A44">
         <f>_xlfn.STDEV.S(extinction!A162:A171)</f>
         <v>0</v>
@@ -6940,8 +7605,24 @@
         <f>_xlfn.STDEV.S(extinction!AL162:AL171)</f>
         <v>1.2184135357012372E-2</v>
       </c>
+      <c r="AN44">
+        <f>IFERROR(ROUNDUP(AI44,-INT(LOG(AI44))+($AO$54-1)),0)</f>
+        <v>8.3000000000000001E-3</v>
+      </c>
+      <c r="AO44">
+        <f>IFERROR(ROUNDUP(AJ44,-INT(LOG(AJ44))+($AO$54-1)),0)</f>
+        <v>4.4000000000000003E-3</v>
+      </c>
+      <c r="AP44">
+        <f>IFERROR(ROUNDUP(AK44,-INT(LOG(AK44))+($AO$54-1)),0)</f>
+        <v>9.1999999999999998E-3</v>
+      </c>
+      <c r="AQ44">
+        <f>IFERROR(ROUNDUP(AL44,-INT(LOG(AL44))+($AO$54-1)),0)</f>
+        <v>1.3000000000000001E-2</v>
+      </c>
     </row>
-    <row r="45" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A45">
         <f>_xlfn.STDEV.S(extinction!A172:A181)</f>
         <v>0</v>
@@ -7090,8 +7771,24 @@
         <f>_xlfn.STDEV.S(extinction!AL172:AL181)</f>
         <v>7.3485189795961022E-3</v>
       </c>
+      <c r="AN45">
+        <f>IFERROR(ROUNDUP(AI45,-INT(LOG(AI45))+($AO$54-1)),0)</f>
+        <v>5.5000000000000005E-3</v>
+      </c>
+      <c r="AO45">
+        <f>IFERROR(ROUNDUP(AJ45,-INT(LOG(AJ45))+($AO$54-1)),0)</f>
+        <v>3.4999999999999996E-3</v>
+      </c>
+      <c r="AP45">
+        <f>IFERROR(ROUNDUP(AK45,-INT(LOG(AK45))+($AO$54-1)),0)</f>
+        <v>6.6E-3</v>
+      </c>
+      <c r="AQ45">
+        <f>IFERROR(ROUNDUP(AL45,-INT(LOG(AL45))+($AO$54-1)),0)</f>
+        <v>7.4000000000000003E-3</v>
+      </c>
     </row>
-    <row r="46" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A46">
         <f>_xlfn.STDEV.S(extinction!A182:A191)</f>
         <v>0</v>
@@ -7240,8 +7937,24 @@
         <f>_xlfn.STDEV.S(extinction!AL182:AL191)</f>
         <v>4.083158314346508E-3</v>
       </c>
+      <c r="AN46">
+        <f>IFERROR(ROUNDUP(AI46,-INT(LOG(AI46))+($AO$54-1)),0)</f>
+        <v>2.6999999999999997E-3</v>
+      </c>
+      <c r="AO46">
+        <f>IFERROR(ROUNDUP(AJ46,-INT(LOG(AJ46))+($AO$54-1)),0)</f>
+        <v>1.8E-3</v>
+      </c>
+      <c r="AP46">
+        <f>IFERROR(ROUNDUP(AK46,-INT(LOG(AK46))+($AO$54-1)),0)</f>
+        <v>3.3E-3</v>
+      </c>
+      <c r="AQ46">
+        <f>IFERROR(ROUNDUP(AL46,-INT(LOG(AL46))+($AO$54-1)),0)</f>
+        <v>4.1000000000000003E-3</v>
+      </c>
     </row>
-    <row r="47" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A47">
         <f>_xlfn.STDEV.S(extinction!A192:A201)</f>
         <v>0</v>
@@ -7390,8 +8103,24 @@
         <f>_xlfn.STDEV.S(extinction!AL192:AL201)</f>
         <v>1.9939772604563358E-3</v>
       </c>
+      <c r="AN47">
+        <f>IFERROR(ROUNDUP(AI47,-INT(LOG(AI47))+($AO$54-1)),0)</f>
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="AO47">
+        <f>IFERROR(ROUNDUP(AJ47,-INT(LOG(AJ47))+($AO$54-1)),0)</f>
+        <v>1.1000000000000001E-3</v>
+      </c>
+      <c r="AP47">
+        <f>IFERROR(ROUNDUP(AK47,-INT(LOG(AK47))+($AO$54-1)),0)</f>
+        <v>1.4E-3</v>
+      </c>
+      <c r="AQ47">
+        <f>IFERROR(ROUNDUP(AL47,-INT(LOG(AL47))+($AO$54-1)),0)</f>
+        <v>2E-3</v>
+      </c>
     </row>
-    <row r="48" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A48">
         <f>_xlfn.STDEV.S(extinction!A202:A211)</f>
         <v>0</v>
@@ -7540,8 +8269,24 @@
         <f>_xlfn.STDEV.S(extinction!AL202:AL211)</f>
         <v>2.2215407186275214E-2</v>
       </c>
+      <c r="AN48">
+        <f>IFERROR(ROUNDUP(AI48,-INT(LOG(AI48))+($AO$54-1)),0)</f>
+        <v>1.6E-2</v>
+      </c>
+      <c r="AO48">
+        <f>IFERROR(ROUNDUP(AJ48,-INT(LOG(AJ48))+($AO$54-1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AP48">
+        <f>IFERROR(ROUNDUP(AK48,-INT(LOG(AK48))+($AO$54-1)),0)</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="AQ48">
+        <f>IFERROR(ROUNDUP(AL48,-INT(LOG(AL48))+($AO$54-1)),0)</f>
+        <v>2.3E-2</v>
+      </c>
     </row>
-    <row r="49" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A49">
         <f>_xlfn.STDEV.S(extinction!A212:A221)</f>
         <v>0</v>
@@ -7690,8 +8435,24 @@
         <f>_xlfn.STDEV.S(extinction!AL212:AL221)</f>
         <v>1.8993346413173066E-2</v>
       </c>
+      <c r="AN49">
+        <f>IFERROR(ROUNDUP(AI49,-INT(LOG(AI49))+($AO$54-1)),0)</f>
+        <v>1.9E-2</v>
+      </c>
+      <c r="AO49">
+        <f>IFERROR(ROUNDUP(AJ49,-INT(LOG(AJ49))+($AO$54-1)),0)</f>
+        <v>5.2000000000000006E-3</v>
+      </c>
+      <c r="AP49">
+        <f>IFERROR(ROUNDUP(AK49,-INT(LOG(AK49))+($AO$54-1)),0)</f>
+        <v>2.3E-2</v>
+      </c>
+      <c r="AQ49">
+        <f>IFERROR(ROUNDUP(AL49,-INT(LOG(AL49))+($AO$54-1)),0)</f>
+        <v>1.9E-2</v>
+      </c>
     </row>
-    <row r="50" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A50">
         <f>_xlfn.STDEV.S(extinction!A222:A231)</f>
         <v>0</v>
@@ -7840,8 +8601,24 @@
         <f>_xlfn.STDEV.S(extinction!AL222:AL231)</f>
         <v>8.7088135801725482E-3</v>
       </c>
+      <c r="AN50">
+        <f>IFERROR(ROUNDUP(AI50,-INT(LOG(AI50))+($AO$54-1)),0)</f>
+        <v>8.7999999999999988E-3</v>
+      </c>
+      <c r="AO50">
+        <f>IFERROR(ROUNDUP(AJ50,-INT(LOG(AJ50))+($AO$54-1)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="AP50">
+        <f>IFERROR(ROUNDUP(AK50,-INT(LOG(AK50))+($AO$54-1)),0)</f>
+        <v>7.899999999999999E-3</v>
+      </c>
+      <c r="AQ50">
+        <f>IFERROR(ROUNDUP(AL50,-INT(LOG(AL50))+($AO$54-1)),0)</f>
+        <v>8.7999999999999988E-3</v>
+      </c>
     </row>
-    <row r="51" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A51">
         <f>_xlfn.STDEV.S(extinction!A232:A241)</f>
         <v>0</v>
@@ -7990,8 +8767,24 @@
         <f>_xlfn.STDEV.S(extinction!AL232:AL241)</f>
         <v>6.2429243567749329E-3</v>
       </c>
+      <c r="AN51">
+        <f>IFERROR(ROUNDUP(AI51,-INT(LOG(AI51))+($AO$54-1)),0)</f>
+        <v>5.8999999999999999E-3</v>
+      </c>
+      <c r="AO51">
+        <f>IFERROR(ROUNDUP(AJ51,-INT(LOG(AJ51))+($AO$54-1)),0)</f>
+        <v>1E-3</v>
+      </c>
+      <c r="AP51">
+        <f>IFERROR(ROUNDUP(AK51,-INT(LOG(AK51))+($AO$54-1)),0)</f>
+        <v>5.8999999999999999E-3</v>
+      </c>
+      <c r="AQ51">
+        <f>IFERROR(ROUNDUP(AL51,-INT(LOG(AL51))+($AO$54-1)),0)</f>
+        <v>6.3E-3</v>
+      </c>
     </row>
-    <row r="52" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A52">
         <f>_xlfn.STDEV.S(extinction!A242:A251)</f>
         <v>0</v>
@@ -8140,9 +8933,34 @@
         <f>_xlfn.STDEV.S(extinction!AL242:AL251)</f>
         <v>4.6103890366656084E-3</v>
       </c>
+      <c r="AN52">
+        <f>IFERROR(ROUNDUP(AI52,-INT(LOG(AI52))+($AO$54-1)),0)</f>
+        <v>3.5999999999999999E-3</v>
+      </c>
+      <c r="AO52">
+        <f>IFERROR(ROUNDUP(AJ52,-INT(LOG(AJ52))+($AO$54-1)),0)</f>
+        <v>5.2999999999999998E-4</v>
+      </c>
+      <c r="AP52">
+        <f>IFERROR(ROUNDUP(AK52,-INT(LOG(AK52))+($AO$54-1)),0)</f>
+        <v>4.5000000000000005E-3</v>
+      </c>
+      <c r="AQ52">
+        <f>IFERROR(ROUNDUP(AL52,-INT(LOG(AL52))+($AO$54-1)),0)</f>
+        <v>4.7000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AN54" t="s">
+        <v>45</v>
+      </c>
+      <c r="AO54">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -8258,16 +9076,16 @@
         <v>14</v>
       </c>
       <c r="AI1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ1" t="s">
         <v>41</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>42</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>43</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.25">

</xml_diff>